<commit_message>
tagging experiments (works in notebook)
</commit_message>
<xml_diff>
--- a/assets/Overview_training_conditions.xlsx
+++ b/assets/Overview_training_conditions.xlsx
@@ -373,7 +373,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -588,10 +588,10 @@
       <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -606,10 +606,10 @@
       <c r="J5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -621,10 +621,10 @@
       <c r="O5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="7" t="s">
         <v>24</v>
       </c>
       <c r="R5" s="6" t="s">
@@ -1072,7 +1072,54 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="9"/>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
@@ -1080,6 +1127,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B14:Q14">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFFF6D"/>
+        <color rgb="FF77BC65"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>